<commit_message>
Initial commit - Educational Games Website with activity type containers
</commit_message>
<xml_diff>
--- a/Ngoolgab yarrenkoo Miriwoo-biny.xlsx
+++ b/Ngoolgab yarrenkoo Miriwoo-biny.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Miriwoong Language Training and Resources\MLTP (Miriwoong Language Training Program)\Self-paced Modules Project\Current SPM Files\Games Websites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games Websites\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="2265" windowWidth="17280" windowHeight="9960" activeTab="2"/>
+    <workbookView xWindow="2265" yWindow="2265" windowWidth="17280" windowHeight="9960"/>
   </bookViews>
   <sheets>
     <sheet name="Unit 1" sheetId="1" r:id="rId1"/>
     <sheet name="Unit 2" sheetId="2" r:id="rId2"/>
     <sheet name="Unit 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Unit 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="120">
   <si>
     <t>Title</t>
   </si>
@@ -34,34 +35,358 @@
     <t>HTML</t>
   </si>
   <si>
-    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/63dd42a8705847eeb15aed33b438c5c1?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>BE/STAY Present Tense Match-up</t>
-  </si>
-  <si>
-    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/d0b97197f0114b41a0693e021b613cf8?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>Coverb + BE/STAY Present Tense Match-up</t>
-  </si>
-  <si>
-    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/e2826d3e7b954f15a6a03d9859fa73d6?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>Sentence + Location Match-up</t>
-  </si>
-  <si>
-    <t>Thena berrayinga? Write it down.</t>
-  </si>
-  <si>
-    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/d3c47cb422b44ff197ff7a76c7b3ef54?themeId=1&amp;templateId=89&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>Dirrmoong gilijing-ni</t>
-  </si>
-  <si>
-    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/5b61cc283ea64279a0a4ddd28b302052?themeId=4&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Match up</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/d9ee05e4ec4f4661b21b3de4cf834606?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>1.1 Drilling gender using ngenjayinga, ngelayinya</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/a83aed0c648842d6889f0169f69d9307?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>1.2 Drilling gender using ngenjayinga, ngelayinya</t>
+  </si>
+  <si>
+    <t>1.5 Choose the gender</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/7c127524954a4162abb09fd1d4445240?themeId=1&amp;templateId=2&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/e997b720aec04d86b1fd6506027dbf21?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>2.1 BE/STAY present tense</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/983fc70a7c1048979471e004c54231f9?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>2.2 BE/STAY sentences</t>
+  </si>
+  <si>
+    <t>2.3 BE/STAY with places</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/00302fb332654aa5903a73a9f1be5cb4?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/ad425753371d4cbf803e9d5042a4e3fc?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>2.4 Gaboob + BE/STAY Q and A</t>
+  </si>
+  <si>
+    <t>2.5 Locative`</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/b50614864afc40b1a99afdd04f26c9c2?themeId=1&amp;templateId=89&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Type the answer</t>
+  </si>
+  <si>
+    <t>2.6 Gama BE/STAY questions</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/aa552e6ccdce432fab3f8828adcf8641?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>2.7 Gama BE/STAY questions</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/5ea965c0e2414b40a90b86b8763b888c?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>3.1 Spatial adverbs</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/34a466078a554f26a3b95867b576c940?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>3.2 BE/STAY + Locative</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/1d6d20a61b664d2faefc65208bbf6c11?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>3.3.1 BE/STAY + nominal-LOC</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/7e18a310abbd4e61a614b4e2a9c618c4?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.4 Locative inflection </t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/b2c5def57f17493a85f0f6632c114cf5?themeId=1&amp;templateId=89&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.1 BE/STAY tenses</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/72977e04bc3b4af9a6c043a20d9ed068?themeId=1&amp;templateId=2&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.2 Time words</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/0667a1a2438b40679d02e04f328ebdd2?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.3 BE/STAY present</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/089303b8f37e45138a7a41779a3c4367?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.4 BE/STAY past</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/b4ce35949ffc437dab28dd9e19705962?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.5 BE/STAY future</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/994986e612074f5b8519cf384085dfc2?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.6 Woolangem + PAST</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/629580858af64ac288822c30c800e1df?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.7 Jooroongiyam + PAST</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/97e12f72a2384c52b4c181c348b535fc?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.8 Gerleleb + PAST`</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/8c52c4898aee4a9c8dceaafaacac050d?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.9 Gelengoo/gelengiya</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/4e47135b23294f02ac696920581d42ab?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.10 Ngooboorram, geraga, gelengam</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/5c0e67c1bbf740e3965fc2fe9e6c994c?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.11 Things from now</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/b6d4101073fc4bc9a3ed26d0b8408ba5?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/8d092494511e4230a7e43e426bf21ee5?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.12 Traditional things</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/1ec27f73f3b442ee8cf2f471323e4e28?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>4.13 Places around town today</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/0fef5b52c653429bac058b3b25962e57?themeId=1&amp;templateId=3&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>3.3.32 BE/STAY + nominal-LOC</t>
+  </si>
+  <si>
+    <t>Picture scene 1 (unit 1)</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/6ff21632aa3449a5b1295d0dd2ff2c22?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Labelled diagram</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/17f70669fb614a43aba791622ca9d5e1?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/a3c54b0eb03448ad9b14bc14b6a6484e?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/9182c54f4704485088de99fa42f35846?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/b2f51183110a41a69503757b49b066ce?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Picture scene 2 (unit 1)</t>
+  </si>
+  <si>
+    <t>Picture scene 3 (unit 1)</t>
+  </si>
+  <si>
+    <t>Picture scene 4 (unit 1)</t>
+  </si>
+  <si>
+    <t>Picture scene 5 (unit 1)</t>
+  </si>
+  <si>
+    <t>Picture scene 6 (unit 2)</t>
+  </si>
+  <si>
+    <t>Picture scene 7 (unit 2)</t>
+  </si>
+  <si>
+    <t>Picture scene 9 (unit 2)</t>
+  </si>
+  <si>
+    <t>Picture scene 8 (unit 2)</t>
+  </si>
+  <si>
+    <t>Picture scene 10 (unit 2)</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/558884a5266d4a03ba9ee8c90171b53c?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/f3413fe177ce472b923ccfead4065b15?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/c494003943554a0fb352f71c9de8ebaa?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/9148de66adf745b3b09e659c18639f55?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/3b97ce771bca4be699def2a3c13eaaf2?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Picture scene 11 (unit 3)</t>
+  </si>
+  <si>
+    <t>Picture scene 12 (unit 3)</t>
+  </si>
+  <si>
+    <t>Picture scene 13 (unit 3)</t>
+  </si>
+  <si>
+    <t>Picture scene 14 (unit 3)</t>
+  </si>
+  <si>
+    <t>Picture scene 15 (unit 3)</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/65672f73ef6a455281149255960e034e?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/6562471bfa004113ac8117d5c5beeaaa?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/18411df0bb384bf48ecc11c01ff50e27?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/4d3cf1f4ebf04b2fa64d130aa703d9e0?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/5a3aab1a1e6647c1b7c5f9f89b9c54ed?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Picture scene 16</t>
+  </si>
+  <si>
+    <t>Picture scene 17</t>
+  </si>
+  <si>
+    <t>Picture scene 18</t>
+  </si>
+  <si>
+    <t>Picture scene 19</t>
+  </si>
+  <si>
+    <t>Picture scene 20</t>
+  </si>
+  <si>
+    <t>Picture scene 21</t>
+  </si>
+  <si>
+    <t>Picture scene 22</t>
+  </si>
+  <si>
+    <t>Picture scene 23</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/aff15d78856c4716aeed8c235790a2c4?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/184c0153c83a4abcad3d94978c2239bc?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/c308b4b265e94231b5b0feea9b367ebf?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/d9554a09451d43f0862889ec13bc2812?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/fa68d32353694eb0bf6c81b38f5fed7e?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/f0195deaa4be42d983885d5417e7912f?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/4e673497697c4f0187f4ffec25dcaf93?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/a4d4320057114d9488141671036d7569?themeId=1&amp;templateId=22&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/d9ee05e4ec4f4661b21b3de4cf834606?themeId=22&amp;templateId=71&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Balloon pop</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/d9ee05e4ec4f4661b21b3de4cf834606?themeId=1&amp;templateId=11&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Crossword</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/d9ee05e4ec4f4661b21b3de4cf834606?themeId=46&amp;templateId=48&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Flying fruit</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/d9ee05e4ec4f4661b21b3de4cf834606?themeId=1&amp;templateId=8&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Spin the wheel</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/a83aed0c648842d6889f0169f69d9307?themeId=22&amp;templateId=71&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/a83aed0c648842d6889f0169f69d9307?themeId=1&amp;templateId=11&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/a83aed0c648842d6889f0169f69d9307?themeId=27&amp;templateId=82&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style="max-width:100%" src="https://wordwall.net/embed/a83aed0c648842d6889f0169f69d9307?themeId=1&amp;templateId=8&amp;fontStackId=0" width="500" height="380" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
   </si>
 </sst>
 </file>
@@ -382,32 +707,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.28515625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -417,10 +914,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,36 +927,147 @@
     <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -469,32 +1077,401 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" customWidth="1"/>
-    <col min="2" max="2" width="47" customWidth="1"/>
+    <col min="1" max="1" width="47.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="47" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51" style="1" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>